<commit_message>
gave groups the updated abilities too, and turned IP addresses into groups
</commit_message>
<xml_diff>
--- a/io9.com.xlsx
+++ b/io9.com.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
   <si>
     <t>Hostname</t>
   </si>
@@ -104,9 +104,6 @@
     <t>AMAZON-02</t>
   </si>
   <si>
-    <t>unknown</t>
-  </si>
-  <si>
     <t>ns-1146.awsdns-15.org.</t>
   </si>
   <si>
@@ -137,12 +134,15 @@
     <t>1 aspmx.l.google.com.</t>
   </si>
   <si>
-    <t>142.250.111.26</t>
+    <t>142.250.123.27</t>
   </si>
   <si>
     <t>MX</t>
   </si>
   <si>
+    <t>gh-in-f27.1e100.net</t>
+  </si>
+  <si>
     <t>GOOGLE</t>
   </si>
   <si>
@@ -158,19 +158,13 @@
     <t>5 alt1.aspmx.l.google.com.</t>
   </si>
   <si>
-    <t>108.177.12.26</t>
-  </si>
-  <si>
-    <t>ua-in-f26.1e100.net</t>
-  </si>
-  <si>
     <t>5 alt2.aspmx.l.google.com.</t>
   </si>
   <si>
-    <t>64.233.186.26</t>
-  </si>
-  <si>
-    <t>cb-in-f26.1e100.net</t>
+    <t>64.233.186.27</t>
+  </si>
+  <si>
+    <t>cb-in-f27.1e100.net</t>
   </si>
 </sst>
 </file>
@@ -706,7 +700,7 @@
         <v>25</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -716,22 +710,22 @@
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1">
       <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -741,22 +735,22 @@
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1">
       <c r="A6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -766,22 +760,22 @@
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1">
       <c r="A7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -791,20 +785,22 @@
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1">
       <c r="A8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
         <v>39</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -820,7 +816,7 @@
         <v>41</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>42</v>
@@ -829,7 +825,7 @@
         <v>39</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -842,19 +838,19 @@
         <v>43</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>39</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -864,22 +860,22 @@
     </row>
     <row r="11" spans="1:11" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>39</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>

</xml_diff>